<commit_message>
Bajando la data de Población Económicamente Activa en México para intentar usarla como serie SIN ESTACIONALIDAD, y CON TENDENCIA
</commit_message>
<xml_diff>
--- a/Nacimientos_MEX1.xlsx
+++ b/Nacimientos_MEX1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\llell\Documents\MIS\Second_semester\Series_UNAM_HPi5\Series_UNAM_HPi5_gitHub\series_UNAM_gitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f9e6e0322c927b48/Documentos/MIS_UNAM/Segundo_semestre/Series_UNAM_HPi3/Series_UNAM_git/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{ECA8F833-FB84-463F-B902-C1BD05382410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nacimientos_MEX" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -515,52 +515,52 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bom" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Célula de Verificação" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Célula Vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Ênfase1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Ênfase2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Ênfase3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Ênfase4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Ênfase5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Ênfase6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Neutro" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Ruim" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -574,7 +574,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -869,14 +869,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -884,7 +886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>34700</v>
       </c>
@@ -892,7 +894,7 @@
         <v>2750444</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>35065</v>
       </c>
@@ -900,7 +902,7 @@
         <v>2707718</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>35431</v>
       </c>
@@ -908,7 +910,7 @@
         <v>2698425</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>35796</v>
       </c>
@@ -916,7 +918,7 @@
         <v>2668428</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>36161</v>
       </c>
@@ -924,7 +926,7 @@
         <v>2769089</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>36526</v>
       </c>
@@ -932,7 +934,7 @@
         <v>2798339</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>36892</v>
       </c>
@@ -940,7 +942,7 @@
         <v>2767610</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>37257</v>
       </c>
@@ -948,7 +950,7 @@
         <v>2699084</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>37622</v>
       </c>
@@ -956,7 +958,7 @@
         <v>2655894</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>37987</v>
       </c>
@@ -964,7 +966,7 @@
         <v>2625056</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>38353</v>
       </c>
@@ -972,7 +974,7 @@
         <v>2567906</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>38718</v>
       </c>
@@ -980,7 +982,7 @@
         <v>2505939</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>39083</v>
       </c>
@@ -988,7 +990,7 @@
         <v>2655083</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>39448</v>
       </c>
@@ -996,7 +998,7 @@
         <v>2636110</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>39814</v>
       </c>
@@ -1004,7 +1006,7 @@
         <v>2577214</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>40179</v>
       </c>
@@ -1012,7 +1014,7 @@
         <v>2643908</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>40544</v>
       </c>
@@ -1020,7 +1022,7 @@
         <v>2586287</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>40909</v>
       </c>
@@ -1028,7 +1030,7 @@
         <v>2498880</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>41275</v>
       </c>
@@ -1036,7 +1038,7 @@
         <v>2478889</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>41640</v>
       </c>
@@ -1044,7 +1046,7 @@
         <v>2463420</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>42005</v>
       </c>
@@ -1052,7 +1054,7 @@
         <v>2353596</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>42370</v>
       </c>
@@ -1060,7 +1062,7 @@
         <v>2293708</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>42736</v>
       </c>
@@ -1068,7 +1070,7 @@
         <v>2234039</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>43101</v>
       </c>
@@ -1076,7 +1078,7 @@
         <v>2162535</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>43466</v>
       </c>
@@ -1084,7 +1086,7 @@
         <v>2092214</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>43831</v>
       </c>
@@ -1092,7 +1094,7 @@
         <v>1629211</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>44197</v>
       </c>

</xml_diff>